<commit_message>
Tried arbitrarily changing selections in an excel document and saving it to see if it would fix superlinter errors.
Files checked in: DataRepo/example_data/testing_data/accucor_with_multiple_labels/accucor_bad_label.xlsx
</commit_message>
<xml_diff>
--- a/DataRepo/example_data/testing_data/accucor_with_multiple_labels/accucor_bad_label.xlsx
+++ b/DataRepo/example_data/testing_data/accucor_with_multiple_labels/accucor_bad_label.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/Downloads/Web/issue-multilabled-tracer-accucor-load/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-local/TRACEBASE/tracebase/DataRepo/example_data/testing_data/accucor_with_multiple_labels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE4B738-99B0-B549-8C4C-02A5B5A84722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F376C02B-38EA-3D41-A886-EF80F5371D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12700" yWindow="500" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -523,9 +523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1388,9 +1386,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>